<commit_message>
JT & Uses cases
Modif' habituels
</commit_message>
<xml_diff>
--- a/Journaux/Journal de bord.xlsx
+++ b/Journaux/Journal de bord.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="20880" windowHeight="8520"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20880" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de bord" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -32,7 +32,10 @@
     <t>Evénement</t>
   </si>
   <si>
-    <t xml:space="preserve">Demande du CdP de refaire le format les Scénarios car le format n'est pas bon </t>
+    <t>Demande du CdP de refaire les Scénarios car le format n'est pas bon</t>
+  </si>
+  <si>
+    <t>Le CdP m'a indiqué comment re-faire mes uses cases et scénarios. Priorité mise sur le rendu de ceux-ci</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,8 +469,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>43160</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>

</xml_diff>